<commit_message>
fix(lab1): update lab1 report
</commit_message>
<xml_diff>
--- a/lab1/report/2112492 刘修铭 第一次个人作业.xlsx
+++ b/lab1/report/2112492 刘修铭 第一次个人作业.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\刘修铭\南开大学\个人材料\课程\2023-2024 第2学期\软件工程 徐思涵\Software_Engineering\lab1\report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lxmliu2002/Desktop/Software_Engineering/lab1/report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D316604-174A-4381-ACB9-139B098E70E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BEA1BEE-C09C-484D-B9F3-C8AE67AE4795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4440" yWindow="760" windowWidth="25800" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2112492 刘修铭" sheetId="2" r:id="rId1"/>
@@ -128,7 +128,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -355,31 +355,10 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -397,8 +376,29 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -677,49 +677,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="F19" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="30.6640625" customWidth="1"/>
     <col min="2" max="2" width="32" customWidth="1"/>
-    <col min="3" max="3" width="70.58203125" customWidth="1"/>
+    <col min="3" max="3" width="70.5" customWidth="1"/>
     <col min="4" max="4" width="70.33203125" customWidth="1"/>
     <col min="5" max="5" width="76.1640625" customWidth="1"/>
-    <col min="6" max="6" width="71.08203125" customWidth="1"/>
+    <col min="6" max="6" width="71" customWidth="1"/>
     <col min="7" max="7" width="76.1640625" customWidth="1"/>
-    <col min="8" max="8" width="71.08203125" customWidth="1"/>
+    <col min="8" max="8" width="71" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13"/>
-      <c r="B1" s="13"/>
-      <c r="C1" s="25" t="s">
+    <row r="1" spans="1:8" ht="45" customHeight="1">
+      <c r="A1" s="18"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="G1" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="H1" s="12" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="218" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
+    <row r="2" spans="1:8" ht="218" customHeight="1">
+      <c r="A2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="15"/>
+      <c r="B2" s="20"/>
       <c r="C2" s="1"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -727,8 +727,8 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" ht="98" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="21" t="s">
+    <row r="3" spans="1:8" ht="98" customHeight="1">
+      <c r="A3" s="14" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -741,8 +741,8 @@
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
     </row>
-    <row r="4" spans="1:8" ht="100" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="21"/>
+    <row r="4" spans="1:8" ht="100" customHeight="1">
+      <c r="A4" s="14"/>
       <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
@@ -753,8 +753,8 @@
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
     </row>
-    <row r="5" spans="1:8" ht="100" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="21"/>
+    <row r="5" spans="1:8" ht="100" customHeight="1">
+      <c r="A5" s="14"/>
       <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
@@ -765,8 +765,8 @@
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="1:8" ht="100" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="21"/>
+    <row r="6" spans="1:8" ht="100" customHeight="1">
+      <c r="A6" s="14"/>
       <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
@@ -777,8 +777,8 @@
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
     </row>
-    <row r="7" spans="1:8" ht="100" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="21"/>
+    <row r="7" spans="1:8" ht="100" customHeight="1">
+      <c r="A7" s="14"/>
       <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
@@ -789,8 +789,8 @@
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
     </row>
-    <row r="8" spans="1:8" ht="100" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="21"/>
+    <row r="8" spans="1:8" ht="100" customHeight="1">
+      <c r="A8" s="14"/>
       <c r="B8" s="3" t="s">
         <v>7</v>
       </c>
@@ -801,8 +801,8 @@
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
     </row>
-    <row r="9" spans="1:8" ht="100" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="21"/>
+    <row r="9" spans="1:8" ht="100" customHeight="1">
+      <c r="A9" s="14"/>
       <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
@@ -813,8 +813,8 @@
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
     </row>
-    <row r="10" spans="1:8" ht="64" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="22" t="s">
+    <row r="10" spans="1:8" ht="64" customHeight="1">
+      <c r="A10" s="15" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -827,8 +827,8 @@
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
     </row>
-    <row r="11" spans="1:8" ht="100" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="22"/>
+    <row r="11" spans="1:8" ht="100" customHeight="1">
+      <c r="A11" s="15"/>
       <c r="B11" s="5" t="s">
         <v>11</v>
       </c>
@@ -839,8 +839,8 @@
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
     </row>
-    <row r="12" spans="1:8" ht="68" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="22"/>
+    <row r="12" spans="1:8" ht="68" customHeight="1">
+      <c r="A12" s="15"/>
       <c r="B12" s="5" t="s">
         <v>12</v>
       </c>
@@ -851,8 +851,8 @@
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
     </row>
-    <row r="13" spans="1:8" ht="79" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="23" t="s">
+    <row r="13" spans="1:8" ht="79" customHeight="1">
+      <c r="A13" s="16" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="7" t="s">
@@ -865,8 +865,8 @@
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
     </row>
-    <row r="14" spans="1:8" ht="79" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="23"/>
+    <row r="14" spans="1:8" ht="79" customHeight="1">
+      <c r="A14" s="16"/>
       <c r="B14" s="7" t="s">
         <v>15</v>
       </c>
@@ -877,8 +877,8 @@
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
     </row>
-    <row r="15" spans="1:8" ht="62" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="23"/>
+    <row r="15" spans="1:8" ht="62" customHeight="1">
+      <c r="A15" s="16"/>
       <c r="B15" s="7" t="s">
         <v>16</v>
       </c>
@@ -889,8 +889,8 @@
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
     </row>
-    <row r="16" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="23"/>
+    <row r="16" spans="1:8" ht="45" customHeight="1">
+      <c r="A16" s="16"/>
       <c r="B16" s="7" t="s">
         <v>12</v>
       </c>
@@ -901,8 +901,8 @@
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
     </row>
-    <row r="17" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="23"/>
+    <row r="17" spans="1:8" ht="45" customHeight="1">
+      <c r="A17" s="16"/>
       <c r="B17" s="7"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
@@ -911,11 +911,11 @@
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
     </row>
-    <row r="18" spans="1:8" ht="188.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="14" t="s">
+    <row r="18" spans="1:8" ht="188.5" customHeight="1">
+      <c r="A18" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="15"/>
+      <c r="B18" s="20"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -923,8 +923,8 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" ht="210.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="24" t="s">
+    <row r="19" spans="1:8" ht="210.75" customHeight="1">
+      <c r="A19" s="17" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="9" t="s">
@@ -939,8 +939,8 @@
       <c r="G19" s="10"/>
       <c r="H19" s="10"/>
     </row>
-    <row r="20" spans="1:8" ht="210.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="24"/>
+    <row r="20" spans="1:8" ht="210.75" customHeight="1">
+      <c r="A20" s="17"/>
       <c r="B20" s="9" t="s">
         <v>21</v>
       </c>
@@ -953,180 +953,182 @@
       <c r="G20" s="10"/>
       <c r="H20" s="10"/>
     </row>
-    <row r="21" spans="1:8" ht="112.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="16" t="s">
+    <row r="21" spans="1:8" ht="112.25" customHeight="1">
+      <c r="A21" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="17"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-    </row>
-    <row r="22" spans="1:8" ht="216" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="18" t="s">
+      <c r="B21" s="22"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="25"/>
+    </row>
+    <row r="22" spans="1:8" ht="216" customHeight="1">
+      <c r="A22" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="19"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-    </row>
-    <row r="23" spans="1:8" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="A23" s="12"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-    </row>
-    <row r="24" spans="1:8" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="A24" s="12"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-    </row>
-    <row r="25" spans="1:8" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="A25" s="12"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
-    </row>
-    <row r="26" spans="1:8" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="A26" s="12"/>
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-    </row>
-    <row r="27" spans="1:8" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="A27" s="12"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-    </row>
-    <row r="28" spans="1:8" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="A28" s="12"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
-    </row>
-    <row r="29" spans="1:8" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="A29" s="12"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
-    </row>
-    <row r="30" spans="1:8" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="A30" s="12"/>
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
-    </row>
-    <row r="31" spans="1:8" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="A31" s="12"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="12"/>
-      <c r="H31" s="12"/>
-    </row>
-    <row r="32" spans="1:8" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="A32" s="12"/>
-      <c r="B32" s="12"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="12"/>
-      <c r="H32" s="12"/>
-    </row>
-    <row r="33" spans="1:8" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="A33" s="12"/>
-      <c r="B33" s="12"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
-      <c r="G33" s="12"/>
-      <c r="H33" s="12"/>
-    </row>
-    <row r="34" spans="1:8" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="A34" s="12"/>
-      <c r="B34" s="12"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="12"/>
-      <c r="G34" s="12"/>
-      <c r="H34" s="12"/>
-    </row>
-    <row r="35" spans="1:8" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="A35" s="12"/>
-      <c r="B35" s="12"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
-      <c r="G35" s="12"/>
-      <c r="H35" s="12"/>
-    </row>
-    <row r="36" spans="1:8" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="A36" s="12"/>
-      <c r="B36" s="12"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="12"/>
-      <c r="G36" s="12"/>
-      <c r="H36" s="12"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+    </row>
+    <row r="23" spans="1:8" ht="18">
+      <c r="A23" s="11"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+    </row>
+    <row r="24" spans="1:8" ht="18">
+      <c r="A24" s="11"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+    </row>
+    <row r="25" spans="1:8" ht="18">
+      <c r="A25" s="11"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+    </row>
+    <row r="26" spans="1:8" ht="18">
+      <c r="A26" s="11"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+    </row>
+    <row r="27" spans="1:8" ht="18">
+      <c r="A27" s="11"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+    </row>
+    <row r="28" spans="1:8" ht="18">
+      <c r="A28" s="11"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+    </row>
+    <row r="29" spans="1:8" ht="18">
+      <c r="A29" s="11"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+    </row>
+    <row r="30" spans="1:8" ht="18">
+      <c r="A30" s="11"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+    </row>
+    <row r="31" spans="1:8" ht="18">
+      <c r="A31" s="11"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+    </row>
+    <row r="32" spans="1:8" ht="18">
+      <c r="A32" s="11"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+    </row>
+    <row r="33" spans="1:8" ht="18">
+      <c r="A33" s="11"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+    </row>
+    <row r="34" spans="1:8" ht="18">
+      <c r="A34" s="11"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+    </row>
+    <row r="35" spans="1:8" ht="18">
+      <c r="A35" s="11"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+    </row>
+    <row r="36" spans="1:8" ht="18">
+      <c r="A36" s="11"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="A3:A9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A13:A17"/>
-    <mergeCell ref="A19:A20"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A3:A9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="C22:H22"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix(lab1): update lab1 excel
</commit_message>
<xml_diff>
--- a/lab1/report/2112492 刘修铭 第一次个人作业.xlsx
+++ b/lab1/report/2112492 刘修铭 第一次个人作业.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\刘修铭\南开大学\个人材料\课程\2023-2024 第2学期\软件工程 徐思涵\Software_Engineering\lab1\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DCEB1BF-3D00-4E73-B21B-88B813F35456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{844AF1AC-11F5-4FF6-BE3C-77346C7AFF50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="2112492 刘修铭" sheetId="2" r:id="rId1"/>
+    <sheet name="总结" sheetId="3" r:id="rId1"/>
+    <sheet name="详细" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="180">
   <si>
     <t>软件概述</t>
   </si>
@@ -11800,6 +11801,1904 @@
         <sz val="16"/>
         <color theme="1"/>
         <rFont val="微软雅黑"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>是把双刃剑，有好有坏，一切取决于人。</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">GitHub Copilot </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>是由</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> GitHub </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>与</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> OpenAI </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>合作开发的一款代码智能助手。它基于</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> OpenAI </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> GPT </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>技术，通过深度学习和自然语言处理，能够为开发者提供即时的代码补全建议。</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Tabnine </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>是一款基于机器学习的智能代码补全工具。它能够通过分析代码库和上下文，建立索引并找到统计模式，以根据</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>**</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>开发者自己编写代码的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>**</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>方式创建自定义代码建议。</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Codeium </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>是一款免费、强大的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> AI </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>智能编程助手，能够支持绝大部分主流编程语言和</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> IDE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>，每周会持续更新，具备快速响应和出色的代码建议能力。</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">aiXcoder </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>是一款智能化软件开发助手，能结合上下文为用户生成完整且更符合实际场景的代码行或者代码块，同时提供生成代码、自动生成单元测试、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Bug </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>自动修复、代码解释、生成注释等功能。</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Cody </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>是由代码搜索浏览工具</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Sourcegraph </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>推出的一个</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> AI </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>编程助手，通过阅读整个代码库和代码图，帮助开发人员写代码并回答问题。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Cody </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>使用</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Sourcegraph </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>的代码图和大型语言模型（</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>LLMs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>）的组合，以消除人工开发中的繁琐任务并保持开发人员的工作流程。</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>支持，效果好</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>支持，效果存疑，需要手动修正</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>多语言支持</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用体验较好</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>存在部分功能缺失问题</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>生成质量好，但需人工进行选择</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>代码可读性高</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>生成的代码应该经过开发者仔细审查，确保其满足项目的质量和规范要求。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Copilot </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>能够提供帮助，但最终的责任仍然在于开发者。</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>编程全阶段覆盖</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>功能、性能、安全等需求较高</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>训练数据量大，依据开发者风格给出提示，规范性好</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">IDE </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>适配度不相同，工具存在信息泄露风险，生成的代码有时需二次查验</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>与</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> GitHub Copilot </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>不同的是，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">tabnine </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>在补全代码时是一点点补全，而非像</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> GitHub Copilot </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>一样一口气全部展现给用户。</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>传入二进制文件，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">MLM </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>即可对该文件进行分析，生成反汇编代码。</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>不支持</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>支持，效果存疑</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>较前两个工具，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Codeium </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>除了测试用例的末尾缺少分号之外，其余表现较好。</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">多语言支持，多 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">IDE </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>适配</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">代码重构，代码翻译
+</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Bug </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>修复</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">代码审查，代码协作
+</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>目前，我们开放上线的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>“</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>MLM”</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>模型已支持</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 10MB </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>以内的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> x86</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">x64 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> PE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>MACHO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">ELF </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>格式的可执行程序。使用</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> “IDA </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>插件</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>”</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>模式的用户请在注册后由网页端下载</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> IDA </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>插件并获取访问</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> token</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>。
+据内部消息，该工具后期将逐渐支持更多语言如</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> solidity </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>等。</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">配置无难度，但无法使用 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="3"/>
+      </rPr>
+      <t>Chat</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>配置难度较大，较 VS code 麻烦</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">bug </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>较多，交互性较差</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>笔者认为其整体的使用体验偏生硬，不如</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> VS code </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>交互体验好。但是</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Pycharm </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>上的功能与</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> VS code </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>基本一致，不存在功能缺失的问题。</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>Xcode</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>部署复杂度高，交互性差</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">tabnine Chat </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>只在有许可证的开源代码上进行了训练，保证了我们的模型没有在</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> GPL </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>或其他</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> copyleft </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>代码上进行训练。</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Codeium </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>使用了最先进的加密技术，保证用户的代码在传输过程中不会被泄露或篡改。此外，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Codeium </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>还支持本地模式，让用户可以在自己的设备上运行</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> AI Autocomplete</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>，不需要联网或上传代码。</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>按照其功能定位，其瞄准安全分析的学者与从业人员，为相关人员提供更加便利的分析工具。</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>代码提示功能强大，支持超级多的语言，支持主流的编辑器和</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> IDE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>能通过机器学习，记忆你经常写的代码，进行超级全面的提示（中文和符号都可以提示），提示的代码量较大</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>提示太慢，延迟较高，双手赶不上头脑；和认知中的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> AI </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>差距还是很大，无法进行交互性问答；有时提示的代码，变量错乱，莫名其妙</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">* Codeium </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>支持超过</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 70 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>种编程语言和</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 20 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>余主流</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> IDE
+* Codeium </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">能够实时智能提示代码，生成速度快，延时较低，帮助程序员更快地编写代码；能够自动完成代码；可以自动重构代码；内置了调试器，能够帮助程序员快速发现和解决代码中的问题
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">* Codeium </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>支持多种版本控制系统，方便程序员管理和维护代码；还支持多人协作开发，能够提高团队的工作效率</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>适当减少了软件开发人员的简单重复劳动，减少了无关信息干扰；减少了不规范代码的引入；</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">aiXcoder </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>的版本更新速度快；其</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> bug </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>修复功能，能够帮助用户更快地进行</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> bug </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>修复</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">tabnine </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>目前分为基本版、增强版和企业版；虽然代码提示很全，写的也很快，但是要注意提示的有没有问题，不然改</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> bug </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>的时间会超级长；也会存在一些推荐不够精准的情况；这个插件对于</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> CPU </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>的消耗较大</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Codeium </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>在界面上直接抹去更早的信息，导致</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>“</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>记忆错乱</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>”；</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>在一些情况下，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Codeium </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>的运行结果不及预期，而且还会不遵守约束条件，犯非常明显的错误；在国内使用</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Codeium </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>可能会遇到网络问题，导致下载速度慢；在某些情况下，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Codeium</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>可能会提示需要登录，但点击后没有反应；在提示中，中文可能会出现乱码</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>（一）市场应用缺口</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>理解能力、应用领域、人才培养、商业化、融合程度</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>（二）工具开发设计</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+1. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>作为新上任的项目经理，笔者会从以下几个方面考虑提升</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> AI </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>智能编程助手的竞争力：增强理解能力、扩大应用领域、提高用户体验</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>**</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>：优化用户界面和交互设计，使用户在使用</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> AI </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>智能编程助手时有更好的体验。以产品功能为例，笔者会选择设计一个</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>**</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>代码优化</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>**</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>功能。这个功能可以帮助用户自动优化他们的代码，提高代码的运行效率和可读性。笔者选择做这个功能，是因为在编程过程中，代码优化是一个重要但又耗时的环节，而一个靠谱的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> AI </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>智能编程助手可以有效地解决这个问题。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+2. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>如果笔者来开发一款新的智能辅助编程工具，笔者会选择以</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>**SaaS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>（软件即服务）</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>**</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>的形式开发这款产品。用户可以通过网络在任何地方、任何时间使用这款产品，无需下载和安装，降低了用户的使用门槛。在设计这款产品时，我会从以下几个方面考虑：用户需求、功能设计、开发和测试、用户体验、数据安全、持续优化</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>（三）个人意愿</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>未来在生活中、在编程中不可避免地会受到</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> AI </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>影响。于我而言，我会分场合使用</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> AI </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>工具。如果我需要练习编程，那么我会选择关闭辅助工具；当我在完成课程作业时，我会选择开启以帮助我掌握、理解课程作业，进而提高完成度。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">AI </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
         <family val="1"/>
         <charset val="134"/>
       </rPr>
@@ -11812,7 +13711,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -11896,6 +13795,33 @@
       <sz val="16"/>
       <color theme="1"/>
       <name val="微软雅黑"/>
+      <family val="1"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="1"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="134"/>
     </font>
@@ -12049,7 +13975,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -12074,6 +14000,42 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -12111,40 +14073,43 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -12421,11 +14386,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60D7424A-ACC0-4B58-BCDE-96533E06169C}">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -12441,8 +14406,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="25" x14ac:dyDescent="0.3">
-      <c r="A1" s="9"/>
-      <c r="B1" s="9"/>
+      <c r="A1" s="21"/>
+      <c r="B1" s="21"/>
       <c r="C1" s="6" t="s">
         <v>22</v>
       </c>
@@ -12462,475 +14427,1146 @@
         <v>27</v>
       </c>
     </row>
+    <row r="2" spans="1:8" ht="148.5" x14ac:dyDescent="0.3">
+      <c r="A2" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="23"/>
+      <c r="C2" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="43" x14ac:dyDescent="0.3">
+      <c r="A3" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>143</v>
+      </c>
+      <c r="D3" s="42" t="s">
+        <v>155</v>
+      </c>
+      <c r="E3" s="34" t="s">
+        <v>143</v>
+      </c>
+      <c r="F3" s="34" t="s">
+        <v>143</v>
+      </c>
+      <c r="G3" s="34" t="s">
+        <v>143</v>
+      </c>
+      <c r="H3" s="34" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="42.5" x14ac:dyDescent="0.3">
+      <c r="A4" s="29"/>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>143</v>
+      </c>
+      <c r="D4" s="33" t="s">
+        <v>143</v>
+      </c>
+      <c r="E4" s="33" t="s">
+        <v>143</v>
+      </c>
+      <c r="F4" s="33" t="s">
+        <v>143</v>
+      </c>
+      <c r="G4" s="33" t="s">
+        <v>143</v>
+      </c>
+      <c r="H4" s="42" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="106" x14ac:dyDescent="0.3">
+      <c r="A5" s="29"/>
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>143</v>
+      </c>
+      <c r="D5" s="33" t="s">
+        <v>143</v>
+      </c>
+      <c r="E5" s="33" t="s">
+        <v>143</v>
+      </c>
+      <c r="F5" s="33" t="s">
+        <v>143</v>
+      </c>
+      <c r="G5" s="33" t="s">
+        <v>143</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="63.5" x14ac:dyDescent="0.3">
+      <c r="A6" s="29"/>
+      <c r="B6" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>143</v>
+      </c>
+      <c r="D6" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="33" t="s">
+        <v>143</v>
+      </c>
+      <c r="F6" s="34" t="s">
+        <v>157</v>
+      </c>
+      <c r="G6" s="33" t="s">
+        <v>143</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="42.5" x14ac:dyDescent="0.3">
+      <c r="A7" s="29"/>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>143</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" s="33" t="s">
+        <v>143</v>
+      </c>
+      <c r="F7" s="33" t="s">
+        <v>143</v>
+      </c>
+      <c r="G7" s="33" t="s">
+        <v>143</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="42.5" x14ac:dyDescent="0.3">
+      <c r="A8" s="29"/>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="34" t="s">
+        <v>144</v>
+      </c>
+      <c r="D8" s="34" t="s">
+        <v>158</v>
+      </c>
+      <c r="E8" s="42" t="s">
+        <v>159</v>
+      </c>
+      <c r="F8" s="34" t="s">
+        <v>158</v>
+      </c>
+      <c r="G8" s="34" t="s">
+        <v>158</v>
+      </c>
+      <c r="H8" s="34" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="128.5" x14ac:dyDescent="0.3">
+      <c r="A9" s="29"/>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="D9" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="E9" s="34" t="s">
+        <v>161</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="G9" s="34" t="s">
+        <v>163</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="42.5" x14ac:dyDescent="0.3">
+      <c r="A10" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="35" t="s">
+        <v>146</v>
+      </c>
+      <c r="D10" s="43" t="s">
+        <v>165</v>
+      </c>
+      <c r="E10" s="43" t="s">
+        <v>80</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="64" x14ac:dyDescent="0.3">
+      <c r="A11" s="30"/>
+      <c r="B11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="35" t="s">
+        <v>147</v>
+      </c>
+      <c r="D11" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="E11" s="43" t="s">
+        <v>167</v>
+      </c>
+      <c r="F11" s="18"/>
+      <c r="G11" s="43" t="s">
+        <v>168</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="88.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="30"/>
+      <c r="B12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="43" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="107" x14ac:dyDescent="0.3">
+      <c r="A13" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="36" t="s">
+        <v>148</v>
+      </c>
+      <c r="D13" s="36" t="s">
+        <v>148</v>
+      </c>
+      <c r="E13" s="36" t="s">
+        <v>148</v>
+      </c>
+      <c r="F13" s="36" t="s">
+        <v>148</v>
+      </c>
+      <c r="G13" s="36" t="s">
+        <v>148</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="63.5" x14ac:dyDescent="0.3">
+      <c r="A14" s="31"/>
+      <c r="B14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="36" t="s">
+        <v>149</v>
+      </c>
+      <c r="D14" s="36" t="s">
+        <v>149</v>
+      </c>
+      <c r="E14" s="36" t="s">
+        <v>149</v>
+      </c>
+      <c r="F14" s="36" t="s">
+        <v>149</v>
+      </c>
+      <c r="G14" s="36" t="s">
+        <v>149</v>
+      </c>
+      <c r="H14" s="14" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="85.5" x14ac:dyDescent="0.3">
+      <c r="A15" s="31"/>
+      <c r="B15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="37" t="s">
+        <v>150</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="G15" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="H15" s="14" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="63.5" x14ac:dyDescent="0.3">
+      <c r="A16" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="38" t="s">
+        <v>151</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="E16" s="38" t="s">
+        <v>151</v>
+      </c>
+      <c r="F16" s="38" t="s">
+        <v>151</v>
+      </c>
+      <c r="G16" s="38" t="s">
+        <v>151</v>
+      </c>
+      <c r="H16" s="39" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="25.5" x14ac:dyDescent="0.3">
+      <c r="A17" s="28"/>
+      <c r="B17" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="39" t="s">
+        <v>152</v>
+      </c>
+      <c r="D17" s="39" t="s">
+        <v>152</v>
+      </c>
+      <c r="E17" s="39" t="s">
+        <v>152</v>
+      </c>
+      <c r="F17" s="39" t="s">
+        <v>152</v>
+      </c>
+      <c r="G17" s="39" t="s">
+        <v>152</v>
+      </c>
+      <c r="H17" s="39" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="148.5" x14ac:dyDescent="0.3">
+      <c r="A18" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="40" t="s">
+        <v>153</v>
+      </c>
+      <c r="D18" s="44" t="s">
+        <v>173</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="F18" s="44" t="s">
+        <v>176</v>
+      </c>
+      <c r="G18" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="H18" s="16" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="144" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="32"/>
+      <c r="B19" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="41" t="s">
+        <v>154</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="F19" s="44" t="s">
+        <v>174</v>
+      </c>
+      <c r="G19" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="H19" s="16" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="191.5" x14ac:dyDescent="0.3">
+      <c r="A20" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="25"/>
+      <c r="C20" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="230" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="27"/>
+      <c r="C21" s="45" t="s">
+        <v>179</v>
+      </c>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+    </row>
+    <row r="22" spans="1:8" ht="17.5" x14ac:dyDescent="0.3">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+    </row>
+    <row r="23" spans="1:8" ht="17.5" x14ac:dyDescent="0.3">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+    </row>
+    <row r="24" spans="1:8" ht="17.5" x14ac:dyDescent="0.3">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+    </row>
+    <row r="25" spans="1:8" ht="17.5" x14ac:dyDescent="0.3">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+    </row>
+    <row r="26" spans="1:8" ht="17.5" x14ac:dyDescent="0.3">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+    </row>
+    <row r="27" spans="1:8" ht="17.5" x14ac:dyDescent="0.3">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+    </row>
+    <row r="28" spans="1:8" ht="17.5" x14ac:dyDescent="0.3">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+    </row>
+    <row r="29" spans="1:8" ht="17.5" x14ac:dyDescent="0.3">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+    </row>
+    <row r="30" spans="1:8" ht="17.5" x14ac:dyDescent="0.3">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+    </row>
+    <row r="31" spans="1:8" ht="17.5" x14ac:dyDescent="0.3">
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+    </row>
+    <row r="32" spans="1:8" ht="17.5" x14ac:dyDescent="0.3">
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+    </row>
+    <row r="33" spans="1:8" ht="17.5" x14ac:dyDescent="0.3">
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+    </row>
+    <row r="34" spans="1:8" ht="17.5" x14ac:dyDescent="0.3">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+    </row>
+    <row r="35" spans="1:8" ht="17.5" x14ac:dyDescent="0.3">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:H21"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:A9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="A13:A15"/>
+  </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H35"/>
+  <sheetViews>
+    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="30.6640625" customWidth="1"/>
+    <col min="2" max="2" width="32" customWidth="1"/>
+    <col min="3" max="3" width="70.58203125" customWidth="1"/>
+    <col min="4" max="4" width="70.33203125" customWidth="1"/>
+    <col min="5" max="5" width="76.1640625" customWidth="1"/>
+    <col min="6" max="6" width="71.08203125" customWidth="1"/>
+    <col min="7" max="7" width="76.1640625" customWidth="1"/>
+    <col min="8" max="8" width="71.08203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="25" x14ac:dyDescent="0.3">
+      <c r="A1" s="21"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
     <row r="2" spans="1:8" ht="218" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="24" t="s">
+      <c r="B2" s="23"/>
+      <c r="C2" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="G2" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="H2" s="12" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="104" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="29" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="26" t="s">
+      <c r="F3" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="G3" s="26" t="s">
+      <c r="G3" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="H3" s="26" t="s">
+      <c r="H3" s="13" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="148" x14ac:dyDescent="0.3">
-      <c r="A4" s="17"/>
+      <c r="A4" s="29"/>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D4" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="26" t="s">
+      <c r="E4" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="F4" s="26" t="s">
+      <c r="F4" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="G4" s="26" t="s">
+      <c r="G4" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="H4" s="26" t="s">
+      <c r="H4" s="13" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="192.5" x14ac:dyDescent="0.3">
-      <c r="A5" s="17"/>
+      <c r="A5" s="29"/>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="E5" s="26" t="s">
+      <c r="E5" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="F5" s="26" t="s">
+      <c r="F5" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="26" t="s">
+      <c r="G5" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="H5" s="26" t="s">
+      <c r="H5" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="212" x14ac:dyDescent="0.3">
-      <c r="A6" s="17"/>
+      <c r="A6" s="29"/>
       <c r="B6" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="26" t="s">
+      <c r="D6" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="E6" s="26" t="s">
+      <c r="E6" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="F6" s="26" t="s">
+      <c r="F6" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="G6" s="26" t="s">
+      <c r="G6" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="H6" s="26" t="s">
+      <c r="H6" s="13" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="84" x14ac:dyDescent="0.3">
-      <c r="A7" s="17"/>
+      <c r="A7" s="29"/>
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="D7" s="26" t="s">
+      <c r="D7" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="E7" s="26" t="s">
+      <c r="E7" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="F7" s="26" t="s">
+      <c r="F7" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="G7" s="26" t="s">
+      <c r="G7" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="H7" s="26" t="s">
+      <c r="H7" s="13" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="170" x14ac:dyDescent="0.3">
-      <c r="A8" s="17"/>
+      <c r="A8" s="29"/>
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="D8" s="26" t="s">
+      <c r="D8" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="E8" s="26" t="s">
+      <c r="E8" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="F8" s="26" t="s">
+      <c r="F8" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="G8" s="26" t="s">
+      <c r="G8" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="H8" s="26" t="s">
+      <c r="H8" s="13" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="191.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="17"/>
+      <c r="A9" s="29"/>
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="D9" s="26" t="s">
+      <c r="D9" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="E9" s="26" t="s">
+      <c r="E9" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="F9" s="26" t="s">
+      <c r="F9" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="G9" s="26" t="s">
+      <c r="G9" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="H9" s="26" t="s">
+      <c r="H9" s="13" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="128" x14ac:dyDescent="0.3">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="30" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D10" s="27" t="s">
+      <c r="D10" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="E10" s="27" t="s">
+      <c r="E10" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="F10" s="28" t="s">
+      <c r="F10" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="G10" s="27" t="s">
+      <c r="G10" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="H10" s="27" t="s">
+      <c r="H10" s="9" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="191.5" x14ac:dyDescent="0.3">
-      <c r="A11" s="18"/>
+      <c r="A11" s="30"/>
       <c r="B11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="27" t="s">
+      <c r="C11" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D11" s="27" t="s">
+      <c r="D11" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="E11" s="27" t="s">
+      <c r="E11" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="F11" s="29"/>
-      <c r="G11" s="27" t="s">
+      <c r="F11" s="18"/>
+      <c r="G11" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="H11" s="27" t="s">
+      <c r="H11" s="9" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="169" x14ac:dyDescent="0.3">
-      <c r="A12" s="18"/>
+      <c r="A12" s="30"/>
       <c r="B12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27" t="s">
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27" t="s">
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="297.5" x14ac:dyDescent="0.3">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="31" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="30" t="s">
+      <c r="C13" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="D13" s="30" t="s">
+      <c r="D13" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="E13" s="30" t="s">
+      <c r="E13" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="F13" s="30" t="s">
+      <c r="F13" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="G13" s="30" t="s">
+      <c r="G13" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="H13" s="30" t="s">
+      <c r="H13" s="14" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="276" x14ac:dyDescent="0.3">
-      <c r="A14" s="19"/>
+      <c r="A14" s="31"/>
       <c r="B14" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="30" t="s">
+      <c r="C14" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="D14" s="30" t="s">
+      <c r="D14" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="E14" s="30" t="s">
+      <c r="E14" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="F14" s="30" t="s">
+      <c r="F14" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="G14" s="30" t="s">
+      <c r="G14" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="H14" s="30" t="s">
+      <c r="H14" s="14" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="191.5" x14ac:dyDescent="0.3">
-      <c r="A15" s="19"/>
+      <c r="A15" s="31"/>
       <c r="B15" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="30" t="s">
+      <c r="C15" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="D15" s="30" t="s">
+      <c r="D15" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="E15" s="30" t="s">
+      <c r="E15" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="F15" s="30" t="s">
+      <c r="F15" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="G15" s="30" t="s">
+      <c r="G15" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="H15" s="30" t="s">
+      <c r="H15" s="14" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="380.5" x14ac:dyDescent="0.3">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="28" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="31" t="s">
+      <c r="C16" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="D16" s="31" t="s">
+      <c r="D16" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="E16" s="31" t="s">
+      <c r="E16" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="F16" s="31" t="s">
+      <c r="F16" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="G16" s="31" t="s">
+      <c r="G16" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="H16" s="31" t="s">
+      <c r="H16" s="15" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="409.5" x14ac:dyDescent="0.3">
-      <c r="A17" s="16"/>
+      <c r="A17" s="28"/>
       <c r="B17" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="31" t="s">
+      <c r="C17" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="D17" s="31" t="s">
+      <c r="D17" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="E17" s="31" t="s">
+      <c r="E17" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="F17" s="31" t="s">
+      <c r="F17" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="G17" s="31" t="s">
+      <c r="G17" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="H17" s="31" t="s">
+      <c r="H17" s="15" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="192.5" x14ac:dyDescent="0.3">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="32" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="32" t="s">
+      <c r="C18" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="D18" s="32" t="s">
+      <c r="D18" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="E18" s="32" t="s">
+      <c r="E18" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="F18" s="32" t="s">
+      <c r="F18" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="G18" s="32" t="s">
+      <c r="G18" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="H18" s="32" t="s">
+      <c r="H18" s="16" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="318" x14ac:dyDescent="0.3">
-      <c r="A19" s="20"/>
+      <c r="A19" s="32"/>
       <c r="B19" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="32" t="s">
+      <c r="C19" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="D19" s="32" t="s">
+      <c r="D19" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="E19" s="32" t="s">
+      <c r="E19" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="F19" s="32" t="s">
+      <c r="F19" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="G19" s="32" t="s">
+      <c r="G19" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="H19" s="32" t="s">
+      <c r="H19" s="16" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="191.5" x14ac:dyDescent="0.3">
-      <c r="A20" s="12" t="s">
+      <c r="A20" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="13"/>
-      <c r="C20" s="23" t="s">
+      <c r="B20" s="25"/>
+      <c r="C20" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="D20" s="23" t="s">
+      <c r="D20" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="E20" s="23" t="s">
+      <c r="E20" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="F20" s="23" t="s">
+      <c r="F20" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="G20" s="23" t="s">
+      <c r="G20" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="H20" s="23" t="s">
+      <c r="H20" s="10" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="216" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="15"/>
-      <c r="C21" s="21" t="s">
+      <c r="B21" s="27"/>
+      <c r="C21" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="D21" s="22"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
     </row>
     <row r="22" spans="1:8" ht="17.5" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>

</xml_diff>